<commit_message>
Modification formulaires de renseignement - Ajout requêtes d'insertion dans la base
</commit_message>
<xml_diff>
--- a/#AUTRES/Formulaires De Renseignement/genius-formulaire-de-renseignement-dut-chimie.xlsx
+++ b/#AUTRES/Formulaires De Renseignement/genius-formulaire-de-renseignement-dut-chimie.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carinefranklin/Documents/IUT COURS/serious game/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOUVEAU\Desktop\Genius\#AUTRES\Formulaires De Renseignement\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67FC0AB-72F1-48B1-8DBF-2DB937A33761}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="14040" windowHeight="17540"/>
+    <workbookView xWindow="47880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="111">
   <si>
     <t>Informations de la formation</t>
   </si>
@@ -345,13 +352,28 @@
   </si>
   <si>
     <t>Développement de méthodes d'analyse</t>
+  </si>
+  <si>
+    <t>Id skill :</t>
+  </si>
+  <si>
+    <t>Diplôme</t>
+  </si>
+  <si>
+    <t>Compétence</t>
+  </si>
+  <si>
+    <t>Mission</t>
+  </si>
+  <si>
+    <t>Id diplom :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -361,15 +383,30 @@
       <b/>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -398,7 +435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -406,21 +443,90 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,7 +562,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultPivotStyle="PivotStyleMedium7">
-    <tableStyle name="Sheet1-style" pivot="0" count="2">
+    <tableStyle name="Sheet1-style" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
@@ -473,12 +579,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A10:D14" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A10:D14" headerRowCount="0">
   <tableColumns count="4">
-    <tableColumn id="1" name="Lieu 1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Quartier 1"/>
-    <tableColumn id="4" name="Column4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Lieu 1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Quartier 1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -780,28 +886,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.46484375" style="2" customWidth="1"/>
     <col min="2" max="2" width="34" style="2" customWidth="1"/>
     <col min="3" max="3" width="47" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.796875" style="2" customWidth="1"/>
     <col min="5" max="5" width="33.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" style="2" customWidth="1"/>
-    <col min="7" max="9" width="14.5" style="2"/>
-    <col min="10" max="10" width="23.83203125" style="2" customWidth="1"/>
+    <col min="7" max="9" width="14.46484375" style="2"/>
+    <col min="10" max="10" width="23.796875" style="2" customWidth="1"/>
     <col min="11" max="11" width="33.33203125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="14.5" style="2"/>
+    <col min="12" max="16384" width="14.46484375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -809,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -820,23 +926,35 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
       <c r="I3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>71</v>
       </c>
+      <c r="D4" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="8">
+        <v>7</v>
+      </c>
       <c r="J4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -847,12 +965,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -860,7 +978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
@@ -868,12 +986,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -890,7 +1008,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -907,7 +1025,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -924,7 +1042,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
@@ -941,7 +1059,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
@@ -958,17 +1076,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I15" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J16" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -976,7 +1094,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
@@ -984,13 +1102,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="J19" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="4" t="s">
         <v>38</v>
       </c>
@@ -1001,87 +1119,107 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>80</v>
+      </c>
+      <c r="D21" s="9">
+        <f>E4</f>
+        <v>7</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>81</v>
+      </c>
+      <c r="D22" s="9">
+        <f>E4+1</f>
+        <v>8</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="5" t="s">
         <v>82</v>
+      </c>
+      <c r="D23" s="9">
+        <f>D22+1</f>
+        <v>9</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="5" t="s">
         <v>84</v>
+      </c>
+      <c r="D24" s="9">
+        <f t="shared" ref="D24:D25" si="0">D23+1</f>
+        <v>10</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="5" t="s">
         <v>86</v>
+      </c>
+      <c r="D25" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J26" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I27" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
@@ -1089,7 +1227,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>55</v>
       </c>
@@ -1097,13 +1235,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="J30" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>58</v>
       </c>
@@ -1111,7 +1249,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>41</v>
       </c>
@@ -1122,9 +1260,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="7" t="str">
-        <f t="shared" ref="A33:A37" si="0">B21</f>
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="str">
+        <f t="shared" ref="A33:A37" si="1">B21</f>
         <v>Analyse Chimique</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -1134,9 +1272,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="7" t="str">
-        <f t="shared" si="0"/>
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="str">
+        <f t="shared" si="1"/>
         <v>Synthèse</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1146,9 +1284,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="7" t="str">
-        <f t="shared" si="0"/>
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="str">
+        <f t="shared" si="1"/>
         <v>Qualité</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -1158,9 +1296,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="7" t="str">
-        <f t="shared" si="0"/>
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="str">
+        <f t="shared" si="1"/>
         <v>Communication</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -1170,9 +1308,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="7" t="str">
-        <f t="shared" si="0"/>
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="str">
+        <f t="shared" si="1"/>
         <v>HSE</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -1182,12 +1320,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>41</v>
       </c>
@@ -1201,285 +1339,285 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="5" t="str">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="10">
+        <f>D21</f>
+        <v>7</v>
+      </c>
+      <c r="B41" s="10">
+        <f>D22</f>
+        <v>8</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="10">
+        <f>D21</f>
+        <v>7</v>
+      </c>
+      <c r="B42" s="10">
+        <f>D23</f>
+        <v>9</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="10">
+        <f>D21</f>
+        <v>7</v>
+      </c>
+      <c r="B43" s="10">
+        <f>D24</f>
+        <v>10</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="10">
+        <f>D21</f>
+        <v>7</v>
+      </c>
+      <c r="B44" s="5" t="str">
+        <f t="shared" ref="B44" si="2">B25</f>
+        <v>HSE</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="str">
+        <f t="shared" ref="A45" si="3">B22</f>
+        <v>Synthèse</v>
+      </c>
+      <c r="B45" s="5" t="str">
+        <f t="shared" ref="B45:B46" si="4">B23</f>
+        <v>Qualité</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="str">
+        <f>B22</f>
+        <v>Synthèse</v>
+      </c>
+      <c r="B46" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>Communication</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="10">
+        <f>D22</f>
+        <v>8</v>
+      </c>
+      <c r="B47" s="10">
+        <f>D25</f>
+        <v>11</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="10">
+        <f>D23</f>
+        <v>9</v>
+      </c>
+      <c r="B48" s="5" t="str">
+        <f t="shared" ref="B48" si="5">B24</f>
+        <v>Communication</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="10">
+        <f>D23</f>
+        <v>9</v>
+      </c>
+      <c r="B49" s="10">
+        <f>D25</f>
+        <v>11</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="5" t="str">
+        <f t="shared" ref="A50" si="6">B24</f>
+        <v>Communication</v>
+      </c>
+      <c r="B50" s="5" t="str">
+        <f>B25</f>
+        <v>HSE</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="5" t="str">
         <f>B21</f>
         <v>Analyse Chimique</v>
       </c>
-      <c r="B41" s="7" t="str">
-        <f t="shared" ref="B41:B44" si="1">B22</f>
+      <c r="B54" s="5" t="str">
+        <f>B22</f>
         <v>Synthèse</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="7" t="str">
+      <c r="C54" s="5" t="str">
+        <f>B23</f>
+        <v>Qualité</v>
+      </c>
+      <c r="D54" s="5" t="str">
+        <f t="shared" ref="D54:D55" si="7">B24</f>
+        <v>Communication</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A55" s="5" t="str">
         <f>B21</f>
         <v>Analyse Chimique</v>
       </c>
-      <c r="B42" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="B55" s="5" t="str">
+        <f>B22</f>
+        <v>Synthèse</v>
+      </c>
+      <c r="C55" s="5" t="str">
+        <f t="shared" ref="C55:C56" si="8">B23</f>
         <v>Qualité</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="7" t="str">
+      <c r="D55" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>HSE</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:7" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="str">
         <f>B21</f>
         <v>Analyse Chimique</v>
       </c>
-      <c r="B43" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="B56" s="5" t="str">
+        <f t="shared" ref="B56:B57" si="9">B22</f>
+        <v>Synthèse</v>
+      </c>
+      <c r="C56" s="5" t="str">
+        <f t="shared" si="8"/>
         <v>Communication</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="7" t="str">
-        <f t="shared" ref="A44:A45" si="2">B21</f>
-        <v>Analyse Chimique</v>
-      </c>
-      <c r="B44" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>HSE</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Synthèse</v>
-      </c>
-      <c r="B45" s="7" t="str">
-        <f t="shared" ref="B45:B47" si="3">B23</f>
-        <v>Qualité</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="7" t="str">
-        <f>B22</f>
-        <v>Synthèse</v>
-      </c>
-      <c r="B46" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>Communication</v>
-      </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-    </row>
-    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="7" t="str">
-        <f t="shared" ref="A47:A48" si="4">B22</f>
-        <v>Synthèse</v>
-      </c>
-      <c r="B47" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>HSE</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>Qualité</v>
-      </c>
-      <c r="B48" s="7" t="str">
-        <f t="shared" ref="B48:B49" si="5">B24</f>
-        <v>Communication</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="7" t="str">
-        <f t="shared" ref="A49:A50" si="6">B23</f>
-        <v>Qualité</v>
-      </c>
-      <c r="B49" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>HSE</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>Communication</v>
-      </c>
-      <c r="B50" s="7" t="str">
+      <c r="D56" s="5" t="str">
         <f>B25</f>
         <v>HSE</v>
       </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="7" t="str">
-        <f>B21</f>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:7" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A57" s="5" t="str">
+        <f t="shared" ref="A57:A58" si="10">B21</f>
         <v>Analyse Chimique</v>
       </c>
-      <c r="B54" s="7" t="str">
-        <f>B22</f>
+      <c r="B57" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Qualité</v>
+      </c>
+      <c r="C57" s="5" t="str">
+        <f>B24</f>
+        <v>Communication</v>
+      </c>
+      <c r="D57" s="5" t="str">
+        <f>B25</f>
+        <v>HSE</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A58" s="5" t="str">
+        <f t="shared" si="10"/>
         <v>Synthèse</v>
       </c>
-      <c r="C54" s="7" t="str">
+      <c r="B58" s="5" t="str">
         <f>B23</f>
         <v>Qualité</v>
       </c>
-      <c r="D54" s="7" t="str">
-        <f t="shared" ref="D54:D55" si="7">B24</f>
+      <c r="C58" s="5" t="str">
+        <f>B24</f>
         <v>Communication</v>
       </c>
-      <c r="E54" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="A55" s="7" t="str">
-        <f>B21</f>
-        <v>Analyse Chimique</v>
-      </c>
-      <c r="B55" s="7" t="str">
-        <f>B22</f>
-        <v>Synthèse</v>
-      </c>
-      <c r="C55" s="7" t="str">
-        <f t="shared" ref="C55:C56" si="8">B23</f>
-        <v>Qualité</v>
-      </c>
-      <c r="D55" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>HSE</v>
-      </c>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-    </row>
-    <row r="56" spans="1:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="A56" s="7" t="str">
-        <f>B21</f>
-        <v>Analyse Chimique</v>
-      </c>
-      <c r="B56" s="7" t="str">
-        <f t="shared" ref="B56:B57" si="9">B22</f>
-        <v>Synthèse</v>
-      </c>
-      <c r="C56" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>Communication</v>
-      </c>
-      <c r="D56" s="7" t="str">
+      <c r="D58" s="5" t="str">
         <f>B25</f>
         <v>HSE</v>
       </c>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-    </row>
-    <row r="57" spans="1:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="A57" s="7" t="str">
-        <f t="shared" ref="A57:A58" si="10">B21</f>
-        <v>Analyse Chimique</v>
-      </c>
-      <c r="B57" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>Qualité</v>
-      </c>
-      <c r="C57" s="7" t="str">
-        <f>B24</f>
-        <v>Communication</v>
-      </c>
-      <c r="D57" s="7" t="str">
-        <f>B25</f>
-        <v>HSE</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="A58" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>Synthèse</v>
-      </c>
-      <c r="B58" s="7" t="str">
-        <f>B23</f>
-        <v>Qualité</v>
-      </c>
-      <c r="C58" s="7" t="str">
-        <f>B24</f>
-        <v>Communication</v>
-      </c>
-      <c r="D58" s="7" t="str">
-        <f>B25</f>
-        <v>HSE</v>
-      </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
     </row>
-    <row r="60" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:7" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>41</v>
       </c>
@@ -1502,7 +1640,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:7" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="str">
         <f>B21</f>
         <v>Analyse Chimique</v>
@@ -1528,6 +1666,249 @@
       </c>
       <c r="G62" s="5" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B65" s="12" t="str">
+        <f>IF(B5="","",CONCATENATE("INSERT INTO diplom (DiplomName) VALUES (""",B5,""");"))</f>
+        <v>INSERT INTO diplom (DiplomName) VALUES ("DUT Chimie");</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" s="9" t="str">
+        <f>IF(B10="","",CONCATENATE("INSERT INTO place (PlaceName) VALUES (""",B10,""");"))</f>
+        <v>INSERT INTO place (PlaceName) VALUES ("Centrale énergétique");</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="13"/>
+      <c r="B67" s="9" t="str">
+        <f t="shared" ref="B67:B70" si="11">IF(B11="","",CONCATENATE("INSERT INTO place (PlaceName) VALUES (""",B11,""");"))</f>
+        <v>INSERT INTO place (PlaceName) VALUES ("Décheterie");</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="14"/>
+      <c r="B68" s="9" t="str">
+        <f t="shared" si="11"/>
+        <v>INSERT INTO place (PlaceName) VALUES ("Laiterie");</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="12"/>
+      <c r="B69" s="7" t="str">
+        <f>IF(B13="","",CONCATENATE("INSERT INTO place (PlaceName) VALUES (""",B13,""");"))</f>
+        <v>INSERT INTO place (PlaceName) VALUES ("Chimie/biologie/procédés");</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="12"/>
+      <c r="B70" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>INSERT INTO place (PlaceName) VALUES ("Port");</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B71" s="7" t="str">
+        <f>IF(B21="","",CONCATENATE("INSERT INTO skill (SkillName, SkillDescription) VALUES (""",B21,""",""",C21,""");"))</f>
+        <v>INSERT INTO skill (SkillName, SkillDescription) VALUES ("Analyse Chimique","Procéder à des analyses chimiques quantitatives et qualitatives.");</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="12"/>
+      <c r="B72" s="7" t="str">
+        <f t="shared" ref="B72:B75" si="12">IF(B22="","",CONCATENATE("INSERT INTO skill (SkillName, SkillDescription) VALUES (""",B22,""",""",C22,""");"))</f>
+        <v>INSERT INTO skill (SkillName, SkillDescription) VALUES ("Synthèse","Réaliser suivant un protocole la synthèse chimique d'un composé.");</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="12"/>
+      <c r="B73" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>INSERT INTO skill (SkillName, SkillDescription) VALUES ("Qualité","Engager une démarche qualité.");</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="12"/>
+      <c r="B74" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>INSERT INTO skill (SkillName, SkillDescription) VALUES ("Communication","Se positionner dans son milieu professionnel.");</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="12"/>
+      <c r="B75" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>INSERT INTO skill (SkillName, SkillDescription) VALUES ("HSE","Travailler dans le respect des consignes d'hygiène, sécurité et environnement.");</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B76" s="12" t="str">
+        <f>CONCATENATE("INSERT INTO mission (MissionName, IDRank, IDSkill1) VALUES (""",B33,""",1,",D21,");")</f>
+        <v>INSERT INTO mission (MissionName, IDRank, IDSkill1) VALUES ("Analyse d'une eau",1,7);</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="12"/>
+      <c r="B77" s="12" t="str">
+        <f t="shared" ref="B77:B80" si="13">CONCATENATE("INSERT INTO mission (MissionName, IDRank, IDSkill1) VALUES (""",B34,""",1,",D22,");")</f>
+        <v>INSERT INTO mission (MissionName, IDRank, IDSkill1) VALUES ("Synthèse d'un polymère",1,8);</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="12"/>
+      <c r="B78" s="12" t="str">
+        <f t="shared" si="13"/>
+        <v>INSERT INTO mission (MissionName, IDRank, IDSkill1) VALUES ("Délivrance d'une certification",1,9);</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="12"/>
+      <c r="B79" s="12" t="str">
+        <f t="shared" si="13"/>
+        <v>INSERT INTO mission (MissionName, IDRank, IDSkill1) VALUES ("Organisation d'une réunion de service",1,10);</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="12"/>
+      <c r="B80" s="12" t="str">
+        <f t="shared" si="13"/>
+        <v>INSERT INTO mission (MissionName, IDRank, IDSkill1) VALUES ("Réalisation d'un plan de gestion des déchets",1,11);</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="12"/>
+      <c r="B81" s="12"/>
+    </row>
+    <row r="82" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="12"/>
+      <c r="B82" s="12" t="str">
+        <f>IF(C41&gt;0,CONCATENATE("INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, AssociatedJob) VALUES (""",C41,""",2,",A41,",",B41,",""",D41,""");"),"")</f>
+        <v>INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, AssociatedJob) VALUES ("Synthèse et caractérisation d'une molécule",2,7,8,"Technicien en synthèse chimique");</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="12"/>
+      <c r="B83" s="12" t="str">
+        <f t="shared" ref="B83:B90" si="14">IF(C42&gt;0,CONCATENATE("INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, AssociatedJob) VALUES (""",C42,""",2,",A42,",",B42,",""",D42,""");"),"")</f>
+        <v>INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, AssociatedJob) VALUES ("Assurance qualité des mesures et la conformité des résultats",2,7,9,"Technicien en contrôle qualité");</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="12"/>
+      <c r="B84" s="12" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, AssociatedJob) VALUES ("Rédaction d'un cahier de laboratoire",2,7,10,"Technicien de laboratoire");</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="12"/>
+      <c r="B85" s="12" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="12"/>
+      <c r="B86" s="12" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="12"/>
+      <c r="B87" s="12" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="12"/>
+      <c r="B88" s="12" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, AssociatedJob) VALUES ("Adaptation des protocoles en fonction de la réglementation",2,8,11,"Technicien recherche et développement");</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="12"/>
+      <c r="B89" s="12" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="12"/>
+      <c r="B90" s="12" t="str">
+        <f t="shared" si="14"/>
+        <v>INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, AssociatedJob) VALUES ("Suivi réglementaire",2,9,11,"Responsable qualité");</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="12"/>
+      <c r="B91" s="12"/>
+    </row>
+    <row r="92" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="12"/>
+      <c r="B92" s="12" t="str">
+        <f>IF(E54&gt;0,CONCATENATE("INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, IDSkill3, IDSkill4, AssociatedJob) VALUES (""",E54,""",3,",D21,",",D22,",",D23,",",D24,",""",F54,""");"),"")</f>
+        <v>INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, IDSkill3, IDSkill4, AssociatedJob) VALUES ("Développement de méthodes d'analyse",3,7,8,9,10,"Responsable R&amp;D");</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="12"/>
+      <c r="B93" s="12" t="str">
+        <f>IF(E55&gt;0,CONCATENATE("INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, IDSkill3, IDSkill4, AssociatedJob) VALUES (""",E55,""",3,",D22,",",D23,",",D24,",",D25,",""",F55,""");"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="12"/>
+      <c r="B94" s="12" t="str">
+        <f>IF(E56&gt;0,CONCATENATE("INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, IDSkill3, IDSkill4, AssociatedJob) VALUES (""",E56,""",3,",D22,",",D23,",",D24,",",D25,",""",F56,""");"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="12"/>
+      <c r="B95" s="12" t="str">
+        <f>IF(E57&gt;0,CONCATENATE("INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, IDSkill3, IDSkill4, AssociatedJob) VALUES (""",E57,""",3,",D22,",",D23,",",D24,",",D25,",""",F57,""");"),"")</f>
+        <v>INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, IDSkill3, IDSkill4, AssociatedJob) VALUES ("Gestion d'équipe de techniciens",3,8,9,10,11,"Chef du pôle analyse");</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="12"/>
+      <c r="B96" s="12" t="str">
+        <f>IF(E58&gt;0,CONCATENATE("INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, IDSkill3, IDSkill4, AssociatedJob) VALUES (""",E58,""",3,",D22,",",D23,",",D24,",",D25,",""",F58,""");"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="12"/>
+      <c r="B97" s="12"/>
+    </row>
+    <row r="98" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="12"/>
+      <c r="B98" s="12" t="str">
+        <f>CONCATENATE("INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, IDSkill3, IDSkill4, IDSkill5, AssociatedJob) VALUES (""",F62,""",4,",D21,",",D22,",",D23,",",D24,",",D25,",""",G62,""");")</f>
+        <v>INSERT INTO mission (MissionName, IDRank, IDSkill1, IDSkill2, IDSkill3, IDSkill4, IDSkill5, AssociatedJob) VALUES ("Gestion d'un laboratoire",4,7,8,9,10,11,"Chef de laboratoire");</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B100" s="12" t="str">
+        <f>CONCATENATE("INSERT INTO exam (ExamName, IDDiplom, IDRank, IDSkillSlot1, IDSkillSlot2, IDSkillSlot3, IDSkillSlot4, IDSkillSlot5) VALUES (""",B5,""",",E3,",4,",D21,",",D22,",",D23,",",D24,",""",D25,""");")</f>
+        <v>INSERT INTO exam (ExamName, IDDiplom, IDRank, IDSkillSlot1, IDSkillSlot2, IDSkillSlot3, IDSkillSlot4, IDSkillSlot5) VALUES ("DUT Chimie",2,4,7,8,9,10,"11");</v>
       </c>
     </row>
   </sheetData>

</xml_diff>